<commit_message>
trying to mend sort
</commit_message>
<xml_diff>
--- a/sample_file.xlsx
+++ b/sample_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BA69C8-5B3E-4A3E-BB8D-3F19E0861FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E15A26-3F47-49A7-B5C7-5911F57825DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>ПУБЛИКАЦИЙ</t>
-  </si>
-  <si>
-    <t>УРОВЕНЬ РИСКА</t>
   </si>
   <si>
     <t>ИЗ НИХ: 
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>Похожих публикаций</t>
+  </si>
+  <si>
+    <t>УРОВЕНЬ МАТЕРИАЛЬНОГО НЕГАТИВА</t>
   </si>
 </sst>
 </file>
@@ -749,7 +749,7 @@
   <dimension ref="A1:L126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -781,7 +781,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="3:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="8"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10" t="s">
@@ -791,16 +791,16 @@
         <v>8</v>
       </c>
       <c r="G3" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="I3" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>9</v>
+      <c r="J3" s="21" t="s">
+        <v>27</v>
       </c>
       <c r="K3" s="12"/>
     </row>
@@ -2544,13 +2544,13 @@
         <v>0</v>
       </c>
       <c r="D2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="F2" s="22" t="s">
         <v>14</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>15</v>
       </c>
       <c r="G2" s="22" t="s">
         <v>5</v>
@@ -2564,16 +2564,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="31" t="s">
         <v>16</v>
-      </c>
-      <c r="F3" s="31" t="s">
-        <v>17</v>
       </c>
       <c r="G3" s="32"/>
       <c r="H3" s="32"/>
@@ -23462,37 +23462,37 @@
         <v>6</v>
       </c>
       <c r="H1" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="J1" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="K1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="L1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="M1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="N1" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="O1" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="27" t="s">
-        <v>27</v>
-      </c>
       <c r="P1" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="29" t="s">
+      <c r="R1" s="29" t="s">
         <v>14</v>
-      </c>
-      <c r="R1" s="29" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="25" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
reworked LLM + sample file
</commit_message>
<xml_diff>
--- a/sample_file.xlsx
+++ b/sample_file.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E15A26-3F47-49A7-B5C7-5911F57825DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D12688-BBF0-42F9-B23D-2C69E0622A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,13 +16,14 @@
     <sheet name="Сводка" sheetId="3" r:id="rId1"/>
     <sheet name="Значимые" sheetId="4" r:id="rId2"/>
     <sheet name="Публикации" sheetId="2" r:id="rId3"/>
+    <sheet name="Анализ" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Объект</t>
   </si>
@@ -72,18 +73,6 @@
     <t>Материальность</t>
   </si>
   <si>
-    <t>негатив</t>
-  </si>
-  <si>
-    <t>значительна</t>
-  </si>
-  <si>
-    <t>материальна</t>
-  </si>
-  <si>
-    <t>СО</t>
-  </si>
-  <si>
     <t>Ссылка на источник</t>
   </si>
   <si>
@@ -109,6 +98,21 @@
   </si>
   <si>
     <t>УРОВЕНЬ МАТЕРИАЛЬНОГО НЕГАТИВА</t>
+  </si>
+  <si>
+    <t>ЗАГОЛОВОК</t>
+  </si>
+  <si>
+    <t>ПРИЗНАК</t>
+  </si>
+  <si>
+    <t>АНАЛИЗ</t>
+  </si>
+  <si>
+    <t>ТЕКСТ НОВОСТИ</t>
+  </si>
+  <si>
+    <t>ЭМИТЕНТ/ОБЪЕКТ</t>
   </si>
 </sst>
 </file>
@@ -299,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -382,6 +386,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -749,7 +771,7 @@
   <dimension ref="A1:L126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -800,7 +822,7 @@
         <v>11</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="K3" s="12"/>
     </row>
@@ -2526,7 +2548,7 @@
   <dimension ref="B2:H1738"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2563,18 +2585,10 @@
       <c r="B3" s="16">
         <v>1</v>
       </c>
-      <c r="C3" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="31" t="s">
-        <v>16</v>
-      </c>
+      <c r="C3" s="32"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="32"/>
       <c r="H3" s="32"/>
     </row>
@@ -23462,28 +23476,28 @@
         <v>6</v>
       </c>
       <c r="H1" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="M1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="N1" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="O1" s="27" t="s">
         <v>22</v>
-      </c>
-      <c r="L1" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="27" t="s">
-        <v>26</v>
       </c>
       <c r="P1" s="29" t="s">
         <v>12</v>
@@ -45238,4 +45252,1664 @@
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7589BA0-57F3-4EB1-B5C1-ECB92923A144}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:L126"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="2" style="2" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="60" style="1" customWidth="1"/>
+    <col min="9" max="9" width="59.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="1.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="3"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+    </row>
+    <row r="2" spans="3:10" s="2" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" spans="3:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="12"/>
+    </row>
+    <row r="4" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="8"/>
+      <c r="D4" s="16">
+        <v>1</v>
+      </c>
+      <c r="E4" s="40"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="8"/>
+      <c r="D5" s="18">
+        <f t="shared" ref="D5:D68" si="0">D4+1</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="40"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="8"/>
+      <c r="D6" s="18">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E6" s="40"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="8"/>
+      <c r="D7" s="18">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E7" s="40"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="8"/>
+      <c r="D8" s="18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E8" s="40"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="8"/>
+      <c r="D9" s="18">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E9" s="40"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="8"/>
+      <c r="D10" s="18">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E10" s="40"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="8"/>
+      <c r="D11" s="18">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E11" s="40"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="8"/>
+      <c r="D12" s="18">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E12" s="40"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="8"/>
+      <c r="D13" s="18">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E13" s="40"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="8"/>
+      <c r="D14" s="18">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E14" s="40"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="12"/>
+    </row>
+    <row r="15" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="8"/>
+      <c r="D15" s="18">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E15" s="40"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="8"/>
+      <c r="D16" s="18">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E16" s="40"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="8"/>
+      <c r="D17" s="18">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E17" s="40"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="8"/>
+      <c r="D18" s="18">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E18" s="40"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="8"/>
+      <c r="D19" s="18">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E19" s="40"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="8"/>
+      <c r="D20" s="18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E20" s="40"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="12"/>
+    </row>
+    <row r="21" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="8"/>
+      <c r="D21" s="18">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E21" s="40"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="12"/>
+    </row>
+    <row r="22" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="8"/>
+      <c r="D22" s="18">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="E22" s="40"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="12"/>
+    </row>
+    <row r="23" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="8"/>
+      <c r="D23" s="18">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E23" s="40"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="12"/>
+    </row>
+    <row r="24" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="8"/>
+      <c r="D24" s="18">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="E24" s="40"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="12"/>
+    </row>
+    <row r="25" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="8"/>
+      <c r="D25" s="18">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="E25" s="40"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="12"/>
+    </row>
+    <row r="26" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="8"/>
+      <c r="D26" s="18">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="E26" s="40"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="12"/>
+    </row>
+    <row r="27" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="8"/>
+      <c r="D27" s="18">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="E27" s="40"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="12"/>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C28" s="8"/>
+      <c r="D28" s="18">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="E28" s="40"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="12"/>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C29" s="8"/>
+      <c r="D29" s="18">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="E29" s="40"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="12"/>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C30" s="8"/>
+      <c r="D30" s="18">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="E30" s="40"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="12"/>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C31" s="8"/>
+      <c r="D31" s="18">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="E31" s="40"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="12"/>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C32" s="8"/>
+      <c r="D32" s="18">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="E32" s="40"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="12"/>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C33" s="8"/>
+      <c r="D33" s="18">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E33" s="40"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="12"/>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C34" s="8"/>
+      <c r="D34" s="18">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="E34" s="40"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="12"/>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C35" s="8"/>
+      <c r="D35" s="18">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="E35" s="40"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="12"/>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C36" s="8"/>
+      <c r="D36" s="18">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="E36" s="40"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="37"/>
+      <c r="I36" s="37"/>
+      <c r="J36" s="12"/>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C37" s="8"/>
+      <c r="D37" s="18">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="E37" s="40"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="12"/>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C38" s="8"/>
+      <c r="D38" s="18">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="E38" s="40"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="12"/>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C39" s="8"/>
+      <c r="D39" s="18">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E39" s="40"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="12"/>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C40" s="8"/>
+      <c r="D40" s="18">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="E40" s="40"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="12"/>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C41" s="8"/>
+      <c r="D41" s="18">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="E41" s="40"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="12"/>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C42" s="8"/>
+      <c r="D42" s="18">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="E42" s="40"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="12"/>
+    </row>
+    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C43" s="8"/>
+      <c r="D43" s="18">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="E43" s="40"/>
+      <c r="F43" s="37"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="37"/>
+      <c r="J43" s="12"/>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C44" s="8"/>
+      <c r="D44" s="18">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="E44" s="40"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="37"/>
+      <c r="J44" s="12"/>
+    </row>
+    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C45" s="8"/>
+      <c r="D45" s="18">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E45" s="40"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="12"/>
+    </row>
+    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C46" s="8"/>
+      <c r="D46" s="18">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="E46" s="40"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="12"/>
+    </row>
+    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C47" s="8"/>
+      <c r="D47" s="18">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="E47" s="40"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="12"/>
+    </row>
+    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C48" s="8"/>
+      <c r="D48" s="18">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="E48" s="40"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="37"/>
+      <c r="J48" s="12"/>
+    </row>
+    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C49" s="8"/>
+      <c r="D49" s="18">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="E49" s="40"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="12"/>
+    </row>
+    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C50" s="8"/>
+      <c r="D50" s="18">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="E50" s="40"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="37"/>
+      <c r="J50" s="12"/>
+    </row>
+    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C51" s="8"/>
+      <c r="D51" s="18">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="E51" s="40"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="37"/>
+      <c r="I51" s="37"/>
+      <c r="J51" s="12"/>
+    </row>
+    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C52" s="8"/>
+      <c r="D52" s="18">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="E52" s="40"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="37"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="37"/>
+      <c r="J52" s="12"/>
+    </row>
+    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C53" s="8"/>
+      <c r="D53" s="18">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="E53" s="40"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="37"/>
+      <c r="J53" s="12"/>
+    </row>
+    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C54" s="8"/>
+      <c r="D54" s="18">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="E54" s="40"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="37"/>
+      <c r="J54" s="12"/>
+    </row>
+    <row r="55" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C55" s="8"/>
+      <c r="D55" s="18">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="E55" s="40"/>
+      <c r="F55" s="37"/>
+      <c r="G55" s="37"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="37"/>
+      <c r="J55" s="12"/>
+    </row>
+    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C56" s="8"/>
+      <c r="D56" s="18">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="E56" s="40"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="37"/>
+      <c r="J56" s="12"/>
+    </row>
+    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C57" s="8"/>
+      <c r="D57" s="18">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="E57" s="40"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="37"/>
+      <c r="J57" s="12"/>
+    </row>
+    <row r="58" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C58" s="8"/>
+      <c r="D58" s="18">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="E58" s="40"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="37"/>
+      <c r="I58" s="37"/>
+      <c r="J58" s="12"/>
+    </row>
+    <row r="59" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C59" s="8"/>
+      <c r="D59" s="18">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="E59" s="40"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="37"/>
+      <c r="J59" s="12"/>
+    </row>
+    <row r="60" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C60" s="8"/>
+      <c r="D60" s="18">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="E60" s="40"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="37"/>
+      <c r="I60" s="37"/>
+      <c r="J60" s="12"/>
+    </row>
+    <row r="61" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C61" s="8"/>
+      <c r="D61" s="18">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="E61" s="40"/>
+      <c r="F61" s="37"/>
+      <c r="G61" s="37"/>
+      <c r="H61" s="37"/>
+      <c r="I61" s="37"/>
+      <c r="J61" s="12"/>
+    </row>
+    <row r="62" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C62" s="8"/>
+      <c r="D62" s="18">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="E62" s="40"/>
+      <c r="F62" s="37"/>
+      <c r="G62" s="37"/>
+      <c r="H62" s="37"/>
+      <c r="I62" s="37"/>
+      <c r="J62" s="12"/>
+    </row>
+    <row r="63" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C63" s="8"/>
+      <c r="D63" s="18">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="E63" s="40"/>
+      <c r="F63" s="37"/>
+      <c r="G63" s="37"/>
+      <c r="H63" s="37"/>
+      <c r="I63" s="37"/>
+      <c r="J63" s="12"/>
+    </row>
+    <row r="64" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C64" s="8"/>
+      <c r="D64" s="18">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="E64" s="40"/>
+      <c r="F64" s="37"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="37"/>
+      <c r="I64" s="37"/>
+      <c r="J64" s="12"/>
+    </row>
+    <row r="65" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C65" s="8"/>
+      <c r="D65" s="18">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="E65" s="40"/>
+      <c r="F65" s="37"/>
+      <c r="G65" s="37"/>
+      <c r="H65" s="37"/>
+      <c r="I65" s="37"/>
+      <c r="J65" s="12"/>
+    </row>
+    <row r="66" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C66" s="8"/>
+      <c r="D66" s="18">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="E66" s="40"/>
+      <c r="F66" s="37"/>
+      <c r="G66" s="37"/>
+      <c r="H66" s="37"/>
+      <c r="I66" s="37"/>
+      <c r="J66" s="12"/>
+    </row>
+    <row r="67" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C67" s="8"/>
+      <c r="D67" s="18">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="E67" s="40"/>
+      <c r="F67" s="37"/>
+      <c r="G67" s="37"/>
+      <c r="H67" s="37"/>
+      <c r="I67" s="37"/>
+      <c r="J67" s="12"/>
+    </row>
+    <row r="68" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C68" s="8"/>
+      <c r="D68" s="18">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="E68" s="40"/>
+      <c r="F68" s="37"/>
+      <c r="G68" s="37"/>
+      <c r="H68" s="37"/>
+      <c r="I68" s="37"/>
+      <c r="J68" s="12"/>
+    </row>
+    <row r="69" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C69" s="8"/>
+      <c r="D69" s="18">
+        <f t="shared" ref="D69:D124" si="1">D68+1</f>
+        <v>66</v>
+      </c>
+      <c r="E69" s="40"/>
+      <c r="F69" s="37"/>
+      <c r="G69" s="37"/>
+      <c r="H69" s="37"/>
+      <c r="I69" s="37"/>
+      <c r="J69" s="12"/>
+    </row>
+    <row r="70" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C70" s="8"/>
+      <c r="D70" s="18">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="E70" s="40"/>
+      <c r="F70" s="37"/>
+      <c r="G70" s="37"/>
+      <c r="H70" s="37"/>
+      <c r="I70" s="37"/>
+      <c r="J70" s="12"/>
+    </row>
+    <row r="71" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C71" s="8"/>
+      <c r="D71" s="18">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="E71" s="40"/>
+      <c r="F71" s="37"/>
+      <c r="G71" s="37"/>
+      <c r="H71" s="37"/>
+      <c r="I71" s="37"/>
+      <c r="J71" s="12"/>
+    </row>
+    <row r="72" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C72" s="8"/>
+      <c r="D72" s="18">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="E72" s="40"/>
+      <c r="F72" s="37"/>
+      <c r="G72" s="37"/>
+      <c r="H72" s="37"/>
+      <c r="I72" s="37"/>
+      <c r="J72" s="12"/>
+    </row>
+    <row r="73" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C73" s="8"/>
+      <c r="D73" s="18">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="E73" s="40"/>
+      <c r="F73" s="37"/>
+      <c r="G73" s="37"/>
+      <c r="H73" s="37"/>
+      <c r="I73" s="37"/>
+      <c r="J73" s="12"/>
+    </row>
+    <row r="74" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C74" s="8"/>
+      <c r="D74" s="18">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="E74" s="40"/>
+      <c r="F74" s="37"/>
+      <c r="G74" s="37"/>
+      <c r="H74" s="37"/>
+      <c r="I74" s="37"/>
+      <c r="J74" s="12"/>
+    </row>
+    <row r="75" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C75" s="8"/>
+      <c r="D75" s="18">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="E75" s="40"/>
+      <c r="F75" s="37"/>
+      <c r="G75" s="37"/>
+      <c r="H75" s="37"/>
+      <c r="I75" s="37"/>
+      <c r="J75" s="12"/>
+    </row>
+    <row r="76" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C76" s="8"/>
+      <c r="D76" s="18">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="E76" s="40"/>
+      <c r="F76" s="37"/>
+      <c r="G76" s="37"/>
+      <c r="H76" s="37"/>
+      <c r="I76" s="37"/>
+      <c r="J76" s="12"/>
+    </row>
+    <row r="77" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C77" s="8"/>
+      <c r="D77" s="18">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="E77" s="40"/>
+      <c r="F77" s="37"/>
+      <c r="G77" s="37"/>
+      <c r="H77" s="37"/>
+      <c r="I77" s="37"/>
+      <c r="J77" s="12"/>
+    </row>
+    <row r="78" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C78" s="8"/>
+      <c r="D78" s="18">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="E78" s="40"/>
+      <c r="F78" s="37"/>
+      <c r="G78" s="37"/>
+      <c r="H78" s="37"/>
+      <c r="I78" s="37"/>
+      <c r="J78" s="12"/>
+    </row>
+    <row r="79" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C79" s="8"/>
+      <c r="D79" s="18">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="E79" s="40"/>
+      <c r="F79" s="37"/>
+      <c r="G79" s="37"/>
+      <c r="H79" s="37"/>
+      <c r="I79" s="37"/>
+      <c r="J79" s="12"/>
+    </row>
+    <row r="80" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C80" s="8"/>
+      <c r="D80" s="18">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="E80" s="40"/>
+      <c r="F80" s="37"/>
+      <c r="G80" s="37"/>
+      <c r="H80" s="37"/>
+      <c r="I80" s="37"/>
+      <c r="J80" s="12"/>
+    </row>
+    <row r="81" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C81" s="8"/>
+      <c r="D81" s="18">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="E81" s="40"/>
+      <c r="F81" s="37"/>
+      <c r="G81" s="37"/>
+      <c r="H81" s="37"/>
+      <c r="I81" s="37"/>
+      <c r="J81" s="12"/>
+    </row>
+    <row r="82" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C82" s="8"/>
+      <c r="D82" s="18">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="E82" s="40"/>
+      <c r="F82" s="37"/>
+      <c r="G82" s="37"/>
+      <c r="H82" s="37"/>
+      <c r="I82" s="37"/>
+      <c r="J82" s="12"/>
+    </row>
+    <row r="83" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C83" s="8"/>
+      <c r="D83" s="18">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="E83" s="40"/>
+      <c r="F83" s="37"/>
+      <c r="G83" s="37"/>
+      <c r="H83" s="37"/>
+      <c r="I83" s="37"/>
+      <c r="J83" s="12"/>
+    </row>
+    <row r="84" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C84" s="8"/>
+      <c r="D84" s="18">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="E84" s="40"/>
+      <c r="F84" s="37"/>
+      <c r="G84" s="37"/>
+      <c r="H84" s="37"/>
+      <c r="I84" s="37"/>
+      <c r="J84" s="12"/>
+    </row>
+    <row r="85" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C85" s="8"/>
+      <c r="D85" s="18">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="E85" s="40"/>
+      <c r="F85" s="37"/>
+      <c r="G85" s="37"/>
+      <c r="H85" s="37"/>
+      <c r="I85" s="37"/>
+      <c r="J85" s="12"/>
+    </row>
+    <row r="86" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C86" s="8"/>
+      <c r="D86" s="18">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="E86" s="40"/>
+      <c r="F86" s="37"/>
+      <c r="G86" s="37"/>
+      <c r="H86" s="37"/>
+      <c r="I86" s="37"/>
+      <c r="J86" s="12"/>
+    </row>
+    <row r="87" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C87" s="8"/>
+      <c r="D87" s="18">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="E87" s="40"/>
+      <c r="F87" s="37"/>
+      <c r="G87" s="37"/>
+      <c r="H87" s="37"/>
+      <c r="I87" s="37"/>
+      <c r="J87" s="12"/>
+    </row>
+    <row r="88" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C88" s="8"/>
+      <c r="D88" s="18">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="E88" s="40"/>
+      <c r="F88" s="37"/>
+      <c r="G88" s="37"/>
+      <c r="H88" s="37"/>
+      <c r="I88" s="37"/>
+      <c r="J88" s="12"/>
+    </row>
+    <row r="89" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C89" s="8"/>
+      <c r="D89" s="18">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="E89" s="40"/>
+      <c r="F89" s="37"/>
+      <c r="G89" s="37"/>
+      <c r="H89" s="37"/>
+      <c r="I89" s="37"/>
+      <c r="J89" s="12"/>
+    </row>
+    <row r="90" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C90" s="8"/>
+      <c r="D90" s="18">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="E90" s="40"/>
+      <c r="F90" s="37"/>
+      <c r="G90" s="37"/>
+      <c r="H90" s="37"/>
+      <c r="I90" s="37"/>
+      <c r="J90" s="12"/>
+    </row>
+    <row r="91" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C91" s="8"/>
+      <c r="D91" s="18">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="E91" s="40"/>
+      <c r="F91" s="37"/>
+      <c r="G91" s="37"/>
+      <c r="H91" s="37"/>
+      <c r="I91" s="37"/>
+      <c r="J91" s="12"/>
+    </row>
+    <row r="92" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C92" s="8"/>
+      <c r="D92" s="18">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="E92" s="40"/>
+      <c r="F92" s="37"/>
+      <c r="G92" s="37"/>
+      <c r="H92" s="37"/>
+      <c r="I92" s="37"/>
+      <c r="J92" s="12"/>
+    </row>
+    <row r="93" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C93" s="8"/>
+      <c r="D93" s="18">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="E93" s="40"/>
+      <c r="F93" s="37"/>
+      <c r="G93" s="37"/>
+      <c r="H93" s="37"/>
+      <c r="I93" s="37"/>
+      <c r="J93" s="12"/>
+    </row>
+    <row r="94" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C94" s="8"/>
+      <c r="D94" s="18">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="E94" s="40"/>
+      <c r="F94" s="37"/>
+      <c r="G94" s="37"/>
+      <c r="H94" s="37"/>
+      <c r="I94" s="37"/>
+      <c r="J94" s="12"/>
+    </row>
+    <row r="95" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C95" s="8"/>
+      <c r="D95" s="18">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="E95" s="40"/>
+      <c r="F95" s="37"/>
+      <c r="G95" s="37"/>
+      <c r="H95" s="37"/>
+      <c r="I95" s="37"/>
+      <c r="J95" s="12"/>
+    </row>
+    <row r="96" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C96" s="8"/>
+      <c r="D96" s="18">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="E96" s="40"/>
+      <c r="F96" s="37"/>
+      <c r="G96" s="37"/>
+      <c r="H96" s="37"/>
+      <c r="I96" s="37"/>
+      <c r="J96" s="12"/>
+    </row>
+    <row r="97" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C97" s="8"/>
+      <c r="D97" s="18">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="E97" s="40"/>
+      <c r="F97" s="37"/>
+      <c r="G97" s="37"/>
+      <c r="H97" s="37"/>
+      <c r="I97" s="37"/>
+      <c r="J97" s="12"/>
+    </row>
+    <row r="98" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C98" s="8"/>
+      <c r="D98" s="18">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="E98" s="40"/>
+      <c r="F98" s="37"/>
+      <c r="G98" s="37"/>
+      <c r="H98" s="37"/>
+      <c r="I98" s="37"/>
+      <c r="J98" s="12"/>
+    </row>
+    <row r="99" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C99" s="8"/>
+      <c r="D99" s="18">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="E99" s="40"/>
+      <c r="F99" s="37"/>
+      <c r="G99" s="37"/>
+      <c r="H99" s="37"/>
+      <c r="I99" s="37"/>
+      <c r="J99" s="12"/>
+    </row>
+    <row r="100" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C100" s="8"/>
+      <c r="D100" s="18">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="E100" s="40"/>
+      <c r="F100" s="37"/>
+      <c r="G100" s="37"/>
+      <c r="H100" s="37"/>
+      <c r="I100" s="37"/>
+      <c r="J100" s="12"/>
+    </row>
+    <row r="101" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C101" s="8"/>
+      <c r="D101" s="18">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="E101" s="40"/>
+      <c r="F101" s="37"/>
+      <c r="G101" s="37"/>
+      <c r="H101" s="37"/>
+      <c r="I101" s="37"/>
+      <c r="J101" s="12"/>
+    </row>
+    <row r="102" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C102" s="8"/>
+      <c r="D102" s="18">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="E102" s="40"/>
+      <c r="F102" s="37"/>
+      <c r="G102" s="37"/>
+      <c r="H102" s="37"/>
+      <c r="I102" s="37"/>
+      <c r="J102" s="12"/>
+    </row>
+    <row r="103" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C103" s="8"/>
+      <c r="D103" s="18">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="E103" s="40"/>
+      <c r="F103" s="37"/>
+      <c r="G103" s="37"/>
+      <c r="H103" s="37"/>
+      <c r="I103" s="37"/>
+      <c r="J103" s="12"/>
+    </row>
+    <row r="104" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C104" s="8"/>
+      <c r="D104" s="18">
+        <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
+      <c r="E104" s="40"/>
+      <c r="F104" s="37"/>
+      <c r="G104" s="37"/>
+      <c r="H104" s="37"/>
+      <c r="I104" s="37"/>
+      <c r="J104" s="12"/>
+    </row>
+    <row r="105" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C105" s="8"/>
+      <c r="D105" s="18">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="E105" s="40"/>
+      <c r="F105" s="37"/>
+      <c r="G105" s="37"/>
+      <c r="H105" s="37"/>
+      <c r="I105" s="37"/>
+      <c r="J105" s="12"/>
+    </row>
+    <row r="106" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C106" s="8"/>
+      <c r="D106" s="18">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+      <c r="E106" s="40"/>
+      <c r="F106" s="37"/>
+      <c r="G106" s="37"/>
+      <c r="H106" s="37"/>
+      <c r="I106" s="37"/>
+      <c r="J106" s="12"/>
+    </row>
+    <row r="107" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C107" s="8"/>
+      <c r="D107" s="18">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="E107" s="40"/>
+      <c r="F107" s="37"/>
+      <c r="G107" s="37"/>
+      <c r="H107" s="37"/>
+      <c r="I107" s="37"/>
+      <c r="J107" s="12"/>
+    </row>
+    <row r="108" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C108" s="8"/>
+      <c r="D108" s="18">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="E108" s="40"/>
+      <c r="F108" s="37"/>
+      <c r="G108" s="37"/>
+      <c r="H108" s="37"/>
+      <c r="I108" s="37"/>
+      <c r="J108" s="12"/>
+    </row>
+    <row r="109" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C109" s="8"/>
+      <c r="D109" s="18">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="E109" s="40"/>
+      <c r="F109" s="37"/>
+      <c r="G109" s="37"/>
+      <c r="H109" s="37"/>
+      <c r="I109" s="37"/>
+      <c r="J109" s="12"/>
+    </row>
+    <row r="110" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C110" s="8"/>
+      <c r="D110" s="18">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="E110" s="40"/>
+      <c r="F110" s="37"/>
+      <c r="G110" s="37"/>
+      <c r="H110" s="37"/>
+      <c r="I110" s="37"/>
+      <c r="J110" s="12"/>
+    </row>
+    <row r="111" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C111" s="8"/>
+      <c r="D111" s="18">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="E111" s="40"/>
+      <c r="F111" s="37"/>
+      <c r="G111" s="37"/>
+      <c r="H111" s="37"/>
+      <c r="I111" s="37"/>
+      <c r="J111" s="12"/>
+    </row>
+    <row r="112" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C112" s="8"/>
+      <c r="D112" s="18">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="E112" s="40"/>
+      <c r="F112" s="37"/>
+      <c r="G112" s="37"/>
+      <c r="H112" s="37"/>
+      <c r="I112" s="37"/>
+      <c r="J112" s="12"/>
+    </row>
+    <row r="113" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C113" s="8"/>
+      <c r="D113" s="18">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="E113" s="40"/>
+      <c r="F113" s="37"/>
+      <c r="G113" s="37"/>
+      <c r="H113" s="37"/>
+      <c r="I113" s="37"/>
+      <c r="J113" s="12"/>
+    </row>
+    <row r="114" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C114" s="8"/>
+      <c r="D114" s="18">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="E114" s="40"/>
+      <c r="F114" s="37"/>
+      <c r="G114" s="37"/>
+      <c r="H114" s="37"/>
+      <c r="I114" s="37"/>
+      <c r="J114" s="12"/>
+    </row>
+    <row r="115" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C115" s="8"/>
+      <c r="D115" s="18">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="E115" s="40"/>
+      <c r="F115" s="37"/>
+      <c r="G115" s="37"/>
+      <c r="H115" s="37"/>
+      <c r="I115" s="37"/>
+      <c r="J115" s="12"/>
+    </row>
+    <row r="116" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C116" s="8"/>
+      <c r="D116" s="18">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="E116" s="40"/>
+      <c r="F116" s="37"/>
+      <c r="G116" s="37"/>
+      <c r="H116" s="37"/>
+      <c r="I116" s="37"/>
+      <c r="J116" s="12"/>
+    </row>
+    <row r="117" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C117" s="8"/>
+      <c r="D117" s="18">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+      <c r="E117" s="40"/>
+      <c r="F117" s="37"/>
+      <c r="G117" s="37"/>
+      <c r="H117" s="37"/>
+      <c r="I117" s="37"/>
+      <c r="J117" s="12"/>
+    </row>
+    <row r="118" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C118" s="8"/>
+      <c r="D118" s="18">
+        <f t="shared" si="1"/>
+        <v>115</v>
+      </c>
+      <c r="E118" s="40"/>
+      <c r="F118" s="37"/>
+      <c r="G118" s="37"/>
+      <c r="H118" s="37"/>
+      <c r="I118" s="37"/>
+      <c r="J118" s="12"/>
+    </row>
+    <row r="119" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C119" s="8"/>
+      <c r="D119" s="18">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="E119" s="40"/>
+      <c r="F119" s="37"/>
+      <c r="G119" s="37"/>
+      <c r="H119" s="37"/>
+      <c r="I119" s="37"/>
+      <c r="J119" s="12"/>
+    </row>
+    <row r="120" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C120" s="8"/>
+      <c r="D120" s="18">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="E120" s="40"/>
+      <c r="F120" s="37"/>
+      <c r="G120" s="37"/>
+      <c r="H120" s="37"/>
+      <c r="I120" s="37"/>
+      <c r="J120" s="12"/>
+    </row>
+    <row r="121" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C121" s="8"/>
+      <c r="D121" s="18">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="E121" s="40"/>
+      <c r="F121" s="37"/>
+      <c r="G121" s="37"/>
+      <c r="H121" s="37"/>
+      <c r="I121" s="37"/>
+      <c r="J121" s="12"/>
+    </row>
+    <row r="122" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C122" s="8"/>
+      <c r="D122" s="18">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
+      <c r="E122" s="40"/>
+      <c r="F122" s="37"/>
+      <c r="G122" s="37"/>
+      <c r="H122" s="37"/>
+      <c r="I122" s="37"/>
+      <c r="J122" s="12"/>
+    </row>
+    <row r="123" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C123" s="8"/>
+      <c r="D123" s="18">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="E123" s="40"/>
+      <c r="F123" s="37"/>
+      <c r="G123" s="37"/>
+      <c r="H123" s="37"/>
+      <c r="I123" s="37"/>
+      <c r="J123" s="12"/>
+    </row>
+    <row r="124" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C124" s="8"/>
+      <c r="D124" s="18">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+      <c r="E124" s="40"/>
+      <c r="F124" s="37"/>
+      <c r="G124" s="37"/>
+      <c r="H124" s="37"/>
+      <c r="I124" s="37"/>
+      <c r="J124" s="12"/>
+    </row>
+    <row r="125" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C125" s="13"/>
+      <c r="D125" s="14"/>
+      <c r="E125" s="38"/>
+      <c r="F125" s="38"/>
+      <c r="G125" s="38"/>
+      <c r="H125" s="38"/>
+      <c r="I125" s="38"/>
+      <c r="J125" s="15"/>
+    </row>
+    <row r="126" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D126" s="3"/>
+      <c r="E126" s="35"/>
+      <c r="F126" s="35"/>
+      <c r="G126" s="35"/>
+      <c r="H126" s="35"/>
+      <c r="I126" s="35"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
gpt-4o + new sample
</commit_message>
<xml_diff>
--- a/sample_file.xlsx
+++ b/sample_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D12688-BBF0-42F9-B23D-2C69E0622A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A4B743-268B-4EDE-8871-A6149E31FFAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Сводка" sheetId="3" r:id="rId1"/>
@@ -770,7 +770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -45261,8 +45261,8 @@
   </sheetPr>
   <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -45274,10 +45274,11 @@
     <col min="5" max="5" width="33.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="18.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="60" style="1" customWidth="1"/>
+    <col min="8" max="8" width="85" style="1" customWidth="1"/>
     <col min="9" max="9" width="59.42578125" style="1" customWidth="1"/>
     <col min="10" max="10" width="1.85546875" style="2" customWidth="1"/>
     <col min="11" max="11" width="24.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>

</xml_diff>